<commit_message>
Cadena de Custodia Actualizada
</commit_message>
<xml_diff>
--- a/AF-P05-G3/Anexos/Anexo 2 - Registro de cadena de custodia.xlsx
+++ b/AF-P05-G3/Anexos/Anexo 2 - Registro de cadena de custodia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3kxhoDark\Desktop\CIBER\AFI\Unidad 4\Proyecto 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3kxhoDark\Desktop\CIBER\Repositorios\G3-ANALISIS-FORENSE\AF-P05-G3\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA4ABEF-5765-44F8-BB00-18DAE47D7B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB700B-9061-486C-9CB8-E52EC07649F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,13 +60,13 @@
     <t>Fecha de la transferencia:</t>
   </si>
   <si>
-    <t>Viernes 5 de Abril de 2024</t>
-  </si>
-  <si>
-    <t>Elaboración de un informe técnico sobre el volcado de memoria del ordenador de Francisco José Jiménez.</t>
-  </si>
-  <si>
     <t>Juan Manuel Cumbrera López</t>
+  </si>
+  <si>
+    <t>Lunes 15 de Abril de 2024</t>
+  </si>
+  <si>
+    <t>Elaboración de un informe técnico sobre el volcado de memoria y la imagen del disco del servidor corporativo comprometido.</t>
   </si>
 </sst>
 </file>
@@ -153,6 +153,27 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -160,27 +181,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,7 +466,7 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -480,124 +480,124 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="2:8" ht="45">
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30">
+      <c r="B9" s="5"/>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="2:8" ht="30">
+      <c r="B10" s="5"/>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="2:8" ht="30">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
     <mergeCell ref="B3:H4"/>
     <mergeCell ref="B5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>